<commit_message>
Fehlerbehebung bei context-dict HH-Satzung
</commit_message>
<xml_diff>
--- a/hhdaten/grunddaten.xlsx
+++ b/hhdaten/grunddaten.xlsx
@@ -8,17 +8,20 @@
   </bookViews>
   <sheets>
     <sheet name="gde" sheetId="1" r:id="rId1"/>
-    <sheet name="EW" sheetId="2" r:id="rId2"/>
-    <sheet name="EW_u20" sheetId="3" r:id="rId3"/>
-    <sheet name="Flaeche" sheetId="4" r:id="rId4"/>
-    <sheet name="LFAGHHJ" sheetId="5" r:id="rId5"/>
+    <sheet name="hhdaten" sheetId="6" r:id="rId2"/>
+    <sheet name="EW" sheetId="2" r:id="rId3"/>
+    <sheet name="EW_u20" sheetId="3" r:id="rId4"/>
+    <sheet name="Flaeche" sheetId="4" r:id="rId5"/>
+    <sheet name="LFAGHHJ" sheetId="5" r:id="rId6"/>
+    <sheet name="JAWerte" sheetId="7" r:id="rId7"/>
+    <sheet name="Tabelle3" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>gdenr</t>
   </si>
@@ -87,13 +90,85 @@
   </si>
   <si>
     <t>Ortsbürgermeister</t>
+  </si>
+  <si>
+    <t>kred_zinslos</t>
+  </si>
+  <si>
+    <t>wg_invest</t>
+  </si>
+  <si>
+    <t>vg</t>
+  </si>
+  <si>
+    <t>hhj</t>
+  </si>
+  <si>
+    <t>grst_a</t>
+  </si>
+  <si>
+    <t>grst_b</t>
+  </si>
+  <si>
+    <t>gewst</t>
+  </si>
+  <si>
+    <t>hust_1</t>
+  </si>
+  <si>
+    <t>hust_2</t>
+  </si>
+  <si>
+    <t>hust_3</t>
+  </si>
+  <si>
+    <t>hust_gef</t>
+  </si>
+  <si>
+    <t>ve_ohne_kredit</t>
+  </si>
+  <si>
+    <t>beschluss_vorjahr</t>
+  </si>
+  <si>
+    <t>beschluss_vorvorjahr</t>
+  </si>
+  <si>
+    <t>ja_vvj_beschluss</t>
+  </si>
+  <si>
+    <t>vvj_abgeschlosse</t>
+  </si>
+  <si>
+    <t>tilg</t>
+  </si>
+  <si>
+    <t>saldo_ordFin</t>
+  </si>
+  <si>
+    <t>saldoErg</t>
+  </si>
+  <si>
+    <t>ek_ab</t>
+  </si>
+  <si>
+    <t>ffs</t>
+  </si>
+  <si>
+    <t>ek_eb</t>
+  </si>
+  <si>
+    <t>fin_eb</t>
+  </si>
+  <si>
+    <t>fin_ab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +179,12 @@
     <font>
       <sz val="11"/>
       <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFA31515"/>
+      <name val="Courier New"/>
       <family val="3"/>
     </font>
   </fonts>
@@ -127,9 +208,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -433,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="A25:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +534,7 @@
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,8 +553,11 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -489,8 +577,11 @@
       <c r="F2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -510,8 +601,11 @@
       <c r="F3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20</v>
       </c>
@@ -531,8 +625,11 @@
       <c r="F4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>30</v>
       </c>
@@ -552,8 +649,11 @@
       <c r="F5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>40</v>
       </c>
@@ -573,8 +673,11 @@
       <c r="F6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>50</v>
       </c>
@@ -594,8 +697,11 @@
       <c r="F7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>60</v>
       </c>
@@ -614,6 +720,9 @@
       </c>
       <c r="F8" t="s">
         <v>22</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -624,13 +733,578 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2020</v>
+      </c>
+      <c r="L2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>2020</v>
+      </c>
+      <c r="L3">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>2020</v>
+      </c>
+      <c r="L4">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>2020</v>
+      </c>
+      <c r="L5">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>2020</v>
+      </c>
+      <c r="L6">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>2020</v>
+      </c>
+      <c r="L7">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>2020</v>
+      </c>
+      <c r="L8">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>2021</v>
+      </c>
+      <c r="L9">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>2021</v>
+      </c>
+      <c r="L10">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>2021</v>
+      </c>
+      <c r="L11">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>2021</v>
+      </c>
+      <c r="L12">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>2021</v>
+      </c>
+      <c r="L13">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>50</v>
+      </c>
+      <c r="B14">
+        <v>2021</v>
+      </c>
+      <c r="L14">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>60</v>
+      </c>
+      <c r="B15">
+        <v>2021</v>
+      </c>
+      <c r="L15">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>2022</v>
+      </c>
+      <c r="L16">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>2022</v>
+      </c>
+      <c r="L17">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>2022</v>
+      </c>
+      <c r="L18">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>2022</v>
+      </c>
+      <c r="L19">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>40</v>
+      </c>
+      <c r="B20">
+        <v>2022</v>
+      </c>
+      <c r="L20">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>50</v>
+      </c>
+      <c r="B21">
+        <v>2022</v>
+      </c>
+      <c r="L21">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>60</v>
+      </c>
+      <c r="B22">
+        <v>2022</v>
+      </c>
+      <c r="L22">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>2023</v>
+      </c>
+      <c r="L23">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>2023</v>
+      </c>
+      <c r="C24">
+        <v>510</v>
+      </c>
+      <c r="D24">
+        <v>510</v>
+      </c>
+      <c r="E24">
+        <v>440</v>
+      </c>
+      <c r="F24">
+        <v>48</v>
+      </c>
+      <c r="G24">
+        <f>F24*1.5</f>
+        <v>72</v>
+      </c>
+      <c r="H24">
+        <f>G24*1.5</f>
+        <v>108</v>
+      </c>
+      <c r="I24">
+        <v>480</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>50000</v>
+      </c>
+      <c r="O24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <v>2023</v>
+      </c>
+      <c r="C25">
+        <v>510</v>
+      </c>
+      <c r="D25">
+        <v>510</v>
+      </c>
+      <c r="E25">
+        <v>440</v>
+      </c>
+      <c r="F25">
+        <v>60</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ref="G25:H29" si="0">F25*1.5</f>
+        <v>90</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="I25">
+        <v>480</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>50000</v>
+      </c>
+      <c r="O25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>2023</v>
+      </c>
+      <c r="C26">
+        <v>510</v>
+      </c>
+      <c r="D26">
+        <v>510</v>
+      </c>
+      <c r="E26">
+        <v>440</v>
+      </c>
+      <c r="F26">
+        <v>84</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>189</v>
+      </c>
+      <c r="I26">
+        <v>480</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>50000</v>
+      </c>
+      <c r="O26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>40</v>
+      </c>
+      <c r="B27">
+        <v>2023</v>
+      </c>
+      <c r="C27">
+        <v>510</v>
+      </c>
+      <c r="D27">
+        <v>510</v>
+      </c>
+      <c r="E27">
+        <v>440</v>
+      </c>
+      <c r="F27">
+        <v>144</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>216</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>324</v>
+      </c>
+      <c r="I27">
+        <v>480</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>50000</v>
+      </c>
+      <c r="O27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>50</v>
+      </c>
+      <c r="B28">
+        <v>2023</v>
+      </c>
+      <c r="C28">
+        <v>560</v>
+      </c>
+      <c r="D28">
+        <v>580</v>
+      </c>
+      <c r="E28">
+        <v>440</v>
+      </c>
+      <c r="F28">
+        <v>120</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+      <c r="I28">
+        <v>480</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>50000</v>
+      </c>
+      <c r="O28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>60</v>
+      </c>
+      <c r="B29">
+        <v>2023</v>
+      </c>
+      <c r="C29">
+        <v>510</v>
+      </c>
+      <c r="D29">
+        <v>510</v>
+      </c>
+      <c r="E29">
+        <v>440</v>
+      </c>
+      <c r="F29">
+        <v>72</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>162</v>
+      </c>
+      <c r="I29">
+        <v>480</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>50000</v>
+      </c>
+      <c r="M29" s="3">
+        <v>44541</v>
+      </c>
+      <c r="N29" s="2">
+        <v>44197</v>
+      </c>
+      <c r="O29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -650,9 +1324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -664,10 +1336,326 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="A25:E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2020</v>
+      </c>
+      <c r="I2">
+        <f>C2+E2</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>D2+H2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>50</v>
+      </c>
+      <c r="B14">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>60</v>
+      </c>
+      <c r="B15">
+        <v>2021</v>
+      </c>
+      <c r="C15">
+        <v>10000000</v>
+      </c>
+      <c r="I15">
+        <v>11000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>40</v>
+      </c>
+      <c r="B20">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>50</v>
+      </c>
+      <c r="B21">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>60</v>
+      </c>
+      <c r="B22">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>40</v>
+      </c>
+      <c r="B27">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>50</v>
+      </c>
+      <c r="B28">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>60</v>
+      </c>
+      <c r="B29">
+        <v>2023</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>